<commit_message>
AltriaUS update to code
</commit_message>
<xml_diff>
--- a/Projects/ALTRIAUS_SAND/Data/KENGINE_ALTRIA_V1.xlsx
+++ b/Projects/ALTRIAUS_SAND/Data/KENGINE_ALTRIA_V1.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="KPI" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Spacing" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="21">
   <si>
     <t xml:space="preserve">KPI Level 1 Name</t>
   </si>
@@ -74,6 +75,15 @@
   </si>
   <si>
     <t xml:space="preserve">Cigars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size</t>
   </si>
 </sst>
 </file>
@@ -200,14 +210,15 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3:G5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.0459183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -310,4 +321,269 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>